<commit_message>
added new usb port
</commit_message>
<xml_diff>
--- a/documents/LCD board.xlsx
+++ b/documents/LCD board.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="161">
   <si>
     <t>STM32F4 Pin</t>
   </si>
@@ -457,6 +457,57 @@
   </si>
   <si>
     <t>PD15</t>
+  </si>
+  <si>
+    <t>GPIOE</t>
+  </si>
+  <si>
+    <t>PE0</t>
+  </si>
+  <si>
+    <t>PE1</t>
+  </si>
+  <si>
+    <t>PE2</t>
+  </si>
+  <si>
+    <t>PE3</t>
+  </si>
+  <si>
+    <t>PE4</t>
+  </si>
+  <si>
+    <t>PE5</t>
+  </si>
+  <si>
+    <t>PE6</t>
+  </si>
+  <si>
+    <t>PE7</t>
+  </si>
+  <si>
+    <t>PE8</t>
+  </si>
+  <si>
+    <t>PE9</t>
+  </si>
+  <si>
+    <t>PE10</t>
+  </si>
+  <si>
+    <t>PE11</t>
+  </si>
+  <si>
+    <t>PE12</t>
+  </si>
+  <si>
+    <t>PE13</t>
+  </si>
+  <si>
+    <t>PE14</t>
+  </si>
+  <si>
+    <t>PE15</t>
   </si>
 </sst>
 </file>
@@ -625,14 +676,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -646,12 +700,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -973,7 +1024,7 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -998,24 +1049,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="H1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="H1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -1075,7 +1126,7 @@
         <v>52</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="18" t="s">
         <v>56</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1088,7 +1139,7 @@
       <c r="N3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="16" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1106,7 +1157,7 @@
         <v>52</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="16"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="2" t="s">
         <v>60</v>
       </c>
@@ -1117,7 +1168,7 @@
       <c r="N4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="12"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1133,7 +1184,7 @@
         <v>52</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="17"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="2" t="s">
         <v>61</v>
       </c>
@@ -1144,7 +1195,7 @@
       <c r="N5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="12"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1571,12 +1622,12 @@
       <c r="O22" s="2"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -1588,7 +1639,7 @@
       <c r="C25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="11" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1661,12 +1712,12 @@
       <c r="D30" s="2"/>
     </row>
     <row r="32" spans="1:15" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K32" s="19" t="s">
+      <c r="K32" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -1815,18 +1866,18 @@
       <c r="N35" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="O35" s="20" t="s">
+      <c r="O35" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="P35" s="21" t="s">
+      <c r="P35" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="Q35" s="21" t="s">
+      <c r="Q35" s="13" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="11" t="s">
         <v>132</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -1876,6 +1927,59 @@
       </c>
       <c r="Q36" s="4" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="P37" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q37" s="4" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added resistors and ESD protection to USB
</commit_message>
<xml_diff>
--- a/documents/LCD board.xlsx
+++ b/documents/LCD board.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pins" sheetId="1" r:id="rId1"/>
-    <sheet name="Odd Parts" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Odd Parts" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -1023,7 +1024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -2014,10 +2015,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2055,7 +2068,7 @@
       <c r="A4" t="s">
         <v>111</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2063,6 +2076,7 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B1" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added LED strip schematic
</commit_message>
<xml_diff>
--- a/documents/LCD board.xlsx
+++ b/documents/LCD board.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\auvic\LCD_board\LCD_board\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{95E4C675-5965-4DA9-AE6C-E9A4DBC3534B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pins" sheetId="1" r:id="rId1"/>
@@ -525,7 +526,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -677,6 +678,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -695,14 +701,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1019,7 +1020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1048,24 +1049,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="H1" s="15" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="H1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1125,7 +1126,7 @@
         <v>52</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="19" t="s">
         <v>56</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1138,7 +1139,7 @@
       <c r="N3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="17" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1156,7 +1157,7 @@
         <v>52</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="17"/>
+      <c r="H4" s="20"/>
       <c r="I4" s="2" t="s">
         <v>60</v>
       </c>
@@ -1167,7 +1168,7 @@
       <c r="N4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="14"/>
+      <c r="O4" s="17"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1183,7 +1184,7 @@
         <v>52</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="18"/>
+      <c r="H5" s="21"/>
       <c r="I5" s="2" t="s">
         <v>61</v>
       </c>
@@ -1194,7 +1195,7 @@
       <c r="N5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="14"/>
+      <c r="O5" s="17"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1621,29 +1622,29 @@
       <c r="O22" s="2"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="F24" s="20" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="F24" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="15" t="s">
         <v>116</v>
       </c>
       <c r="F25" s="6" t="s">
@@ -1669,13 +1670,13 @@
       <c r="D26" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="19" t="s">
+      <c r="F26" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="H26" s="19" t="s">
+      <c r="H26" s="13" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1692,13 +1693,13 @@
       <c r="D27" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="13" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2036,11 +2037,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2084,9 +2085,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B1" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
completed most changes in to do.txt
</commit_message>
<xml_diff>
--- a/documents/LCD board.xlsx
+++ b/documents/LCD board.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\auvic\LCD_board\LCD_board\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\AUVIC\LCD_board\LCD_board\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{18E91983-2438-46D5-8000-B3558D4B72B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1BC37092-E474-4AA3-8311-D8600871F900}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1023,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1957,16 +1957,16 @@
       <c r="A37" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>147</v>
       </c>
       <c r="F37" s="4" t="s">

</xml_diff>